<commit_message>
Agrega NB 4_Valorizacion_Sensibilidad.ipynb. Agrega módulo aux_functions.py .
</commit_message>
<xml_diff>
--- a/input/curva_clf.xlsx
+++ b/input/curva_clf.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Procedimientos\help-qc_financial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodiaz/qcf_repos/qcfinancial-help/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5498D312-D5F1-B74F-AF63-1F07D3237C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19180" windowHeight="7600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="5">
-  <si>
-    <t>curva</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>plazo</t>
-  </si>
-  <si>
-    <t>CAMARACLF</t>
   </si>
   <si>
     <t>tasa</t>
@@ -44,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,9 +66,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,488 +347,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-5.6780110000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>-5.6780110000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
+      <c r="B3">
         <v>-5.6744350454600002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>35</v>
       </c>
-      <c r="D4">
+      <c r="B4">
         <v>-9.3399445032000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>64</v>
       </c>
-      <c r="D5">
+      <c r="B5">
         <v>-2.11834077854E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>96</v>
       </c>
-      <c r="D6">
+      <c r="B6">
         <v>-2.0079407425000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>126</v>
       </c>
-      <c r="D7">
+      <c r="B7">
         <v>-2.0761859703099999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>155</v>
       </c>
-      <c r="D8">
+      <c r="B8">
         <v>-1.91973106769E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>188</v>
       </c>
-      <c r="D9">
+      <c r="B9">
         <v>-1.9346540686800001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>218</v>
       </c>
-      <c r="D10">
+      <c r="B10">
         <v>-1.7626365204900001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>249</v>
       </c>
-      <c r="D11">
+      <c r="B11">
         <v>-1.7987076047700001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>279</v>
       </c>
-      <c r="D12">
+      <c r="B12">
         <v>-1.93345971155E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>309</v>
       </c>
-      <c r="D13">
+      <c r="B13">
         <v>-1.8158769468000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>341</v>
       </c>
-      <c r="D14">
+      <c r="B14">
         <v>-1.5939740658499998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>369</v>
       </c>
-      <c r="D15">
+      <c r="B15">
         <v>-1.5994399089500001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>400</v>
       </c>
-      <c r="D16">
+      <c r="B16">
         <v>-1.5067626983500001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>428</v>
       </c>
-      <c r="D17">
+      <c r="B17">
         <v>-1.61147655424E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>461</v>
       </c>
-      <c r="D18">
+      <c r="B18">
         <v>-1.5922893985299998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>491</v>
       </c>
-      <c r="D19">
+      <c r="B19">
         <v>-1.57795744477E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>522</v>
       </c>
-      <c r="D20">
+      <c r="B20">
         <v>-1.51858637768E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>553</v>
       </c>
-      <c r="D21">
+      <c r="B21">
         <v>-1.55333315282E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>582</v>
       </c>
-      <c r="D22">
+      <c r="B22">
         <v>-1.5649056579099999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>734</v>
       </c>
-      <c r="D23">
+      <c r="B23">
         <v>-1.6593660563899999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1099</v>
       </c>
-      <c r="D24">
+      <c r="B24">
         <v>-1.4881085928599999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1465</v>
       </c>
-      <c r="D25">
+      <c r="B25">
         <v>-1.27396873761E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>1830</v>
       </c>
-      <c r="D26">
+      <c r="B26">
         <v>-1.0201214230699999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>2195</v>
       </c>
-      <c r="D27">
+      <c r="B27">
         <v>-8.0085472601300004E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>2560</v>
       </c>
-      <c r="D28">
+      <c r="B28">
         <v>-5.86765288028E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>2926</v>
       </c>
-      <c r="D29">
+      <c r="B29">
         <v>-4.1451913120800002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>3291</v>
       </c>
-      <c r="D30">
+      <c r="B30">
         <v>-3.0466331960400002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>3656</v>
       </c>
-      <c r="D31">
+      <c r="B31">
         <v>-2.2415793656299999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>4387</v>
       </c>
-      <c r="D32">
+      <c r="B32">
         <v>-1.87142850029E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C33">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>5482</v>
       </c>
-      <c r="D33">
+      <c r="B33">
         <v>-1.0562490850199999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="1">
-        <v>43895</v>
-      </c>
-      <c r="C34">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>7309</v>
       </c>
-      <c r="D34">
+      <c r="B34">
         <v>-6.3934691004700005E-4</v>
       </c>
     </row>

</xml_diff>